<commit_message>
feat: Better working model
</commit_message>
<xml_diff>
--- a/OAS2-split.xlsx
+++ b/OAS2-split.xlsx
@@ -657,7 +657,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O4" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>validate</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O6" t="n">
@@ -816,7 +816,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O7" t="n">
@@ -922,7 +922,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>validate</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O9" t="n">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O12" t="n">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O15" t="n">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O16" t="n">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>validate</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O17" t="n">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O19" t="n">
@@ -1770,7 +1770,7 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O25" t="n">
@@ -1876,7 +1876,7 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O27" t="n">
@@ -1982,7 +1982,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O29" t="n">
@@ -2088,7 +2088,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O31" t="n">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O32" t="n">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O33" t="n">
@@ -2459,7 +2459,7 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O38" t="n">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O52" t="n">
@@ -3360,7 +3360,7 @@
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O55" t="n">
@@ -3466,7 +3466,7 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O57" t="n">
@@ -3572,7 +3572,7 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O59" t="n">
@@ -3784,7 +3784,7 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O63" t="n">
@@ -4102,7 +4102,7 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O69" t="n">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>validate</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O72" t="n">
@@ -4526,7 +4526,7 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O77" t="n">
@@ -4897,7 +4897,7 @@
       </c>
       <c r="N84" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O84" t="n">
@@ -5215,7 +5215,7 @@
       </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O90" t="n">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O92" t="n">
@@ -5480,7 +5480,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>validate</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O95" t="n">
@@ -5533,7 +5533,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>validate</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O96" t="n">
@@ -5586,7 +5586,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O97" t="n">
@@ -5692,7 +5692,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O99" t="n">
@@ -5798,7 +5798,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O101" t="n">
@@ -5904,7 +5904,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O103" t="n">
@@ -6169,7 +6169,7 @@
       </c>
       <c r="N108" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O108" t="n">
@@ -6222,7 +6222,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O109" t="n">
@@ -6381,7 +6381,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>validate</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O112" t="n">
@@ -6487,7 +6487,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O114" t="n">
@@ -6540,7 +6540,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O115" t="n">
@@ -6646,7 +6646,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O117" t="n">
@@ -7017,7 +7017,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O124" t="n">
@@ -7123,7 +7123,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O126" t="n">
@@ -7335,7 +7335,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O130" t="n">
@@ -7388,7 +7388,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O131" t="n">
@@ -7441,7 +7441,7 @@
       </c>
       <c r="N132" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O132" t="n">
@@ -7547,7 +7547,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O134" t="n">
@@ -7759,7 +7759,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O138" t="n">
@@ -7812,7 +7812,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O139" t="n">
@@ -7971,7 +7971,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>validate</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O142" t="n">
@@ -8024,7 +8024,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O143" t="n">
@@ -8236,7 +8236,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O147" t="n">
@@ -8395,7 +8395,7 @@
       </c>
       <c r="N150" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O150" t="n">
@@ -8448,7 +8448,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O151" t="n">
@@ -8501,7 +8501,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O152" t="n">
@@ -8660,7 +8660,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O155" t="n">
@@ -8925,7 +8925,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O160" t="n">
@@ -9084,7 +9084,7 @@
       </c>
       <c r="N163" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O163" t="n">
@@ -9508,7 +9508,7 @@
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O171" t="n">
@@ -9720,7 +9720,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O175" t="n">
@@ -10038,7 +10038,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O181" t="n">
@@ -10144,7 +10144,7 @@
       </c>
       <c r="N183" t="inlineStr">
         <is>
-          <t>validate</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O183" t="n">
@@ -10356,7 +10356,7 @@
       </c>
       <c r="N187" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O187" t="n">
@@ -10780,7 +10780,7 @@
       </c>
       <c r="N195" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O195" t="n">
@@ -10939,7 +10939,7 @@
       </c>
       <c r="N198" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O198" t="n">
@@ -11098,7 +11098,7 @@
       </c>
       <c r="N201" t="inlineStr">
         <is>
-          <t>validate</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O201" t="n">
@@ -11946,7 +11946,7 @@
       </c>
       <c r="N217" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O217" t="n">
@@ -12052,7 +12052,7 @@
       </c>
       <c r="N219" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O219" t="n">
@@ -12105,7 +12105,7 @@
       </c>
       <c r="N220" t="inlineStr">
         <is>
-          <t>validate</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O220" t="n">
@@ -12158,7 +12158,7 @@
       </c>
       <c r="N221" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O221" t="n">
@@ -12476,7 +12476,7 @@
       </c>
       <c r="N227" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O227" t="n">
@@ -12900,7 +12900,7 @@
       </c>
       <c r="N235" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O235" t="n">
@@ -12953,7 +12953,7 @@
       </c>
       <c r="N236" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O236" t="n">
@@ -13059,7 +13059,7 @@
       </c>
       <c r="N238" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O238" t="n">
@@ -13165,7 +13165,7 @@
       </c>
       <c r="N240" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O240" t="n">
@@ -13218,7 +13218,7 @@
       </c>
       <c r="N241" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O241" t="n">
@@ -13271,7 +13271,7 @@
       </c>
       <c r="N242" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O242" t="n">
@@ -13377,7 +13377,7 @@
       </c>
       <c r="N244" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O244" t="n">
@@ -13695,7 +13695,7 @@
       </c>
       <c r="N250" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O250" t="n">
@@ -13748,7 +13748,7 @@
       </c>
       <c r="N251" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O251" t="n">
@@ -13907,7 +13907,7 @@
       </c>
       <c r="N254" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O254" t="n">
@@ -13960,7 +13960,7 @@
       </c>
       <c r="N255" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O255" t="n">
@@ -14225,7 +14225,7 @@
       </c>
       <c r="N260" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>test</t>
         </is>
       </c>
       <c r="O260" t="n">
@@ -14384,7 +14384,7 @@
       </c>
       <c r="N263" t="inlineStr">
         <is>
-          <t>validate</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O263" t="n">
@@ -14649,7 +14649,7 @@
       </c>
       <c r="N268" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O268" t="n">
@@ -14861,7 +14861,7 @@
       </c>
       <c r="N272" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O272" t="n">
@@ -15179,7 +15179,7 @@
       </c>
       <c r="N278" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O278" t="n">
@@ -15391,7 +15391,7 @@
       </c>
       <c r="N282" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O282" t="n">
@@ -15497,7 +15497,7 @@
       </c>
       <c r="N284" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O284" t="n">
@@ -15656,7 +15656,7 @@
       </c>
       <c r="N287" t="inlineStr">
         <is>
-          <t>train</t>
+          <t>validate</t>
         </is>
       </c>
       <c r="O287" t="n">
@@ -15762,7 +15762,7 @@
       </c>
       <c r="N289" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>train</t>
         </is>
       </c>
       <c r="O289" t="n">

</xml_diff>